<commit_message>
Risimulate data using pert distribution
</commit_message>
<xml_diff>
--- a/inst/extdata/elicit.xlsx
+++ b/inst/extdata/elicit.xlsx
@@ -404,28 +404,28 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
+        <v>-1</v>
+      </c>
+      <c r="C2" t="n">
+        <v>23</v>
+      </c>
+      <c r="D2" t="n">
+        <v>33</v>
+      </c>
+      <c r="E2" t="n">
+        <v>27</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="G2" t="n">
         <v>0.8</v>
       </c>
-      <c r="C2" t="n">
-        <v>53</v>
-      </c>
-      <c r="D2" t="n">
-        <v>54</v>
-      </c>
-      <c r="E2" t="n">
-        <v>53</v>
-      </c>
-      <c r="F2" t="n">
-        <v>-1</v>
-      </c>
-      <c r="G2" t="n">
-        <v>-6</v>
-      </c>
       <c r="H2" t="n">
-        <v>-1</v>
+        <v>0.6</v>
       </c>
       <c r="I2" t="n">
-        <v>89</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3">
@@ -433,28 +433,28 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>0.9</v>
+        <v>-5</v>
       </c>
       <c r="C3" t="n">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="D3" t="n">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="E3" t="n">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="F3" t="n">
-        <v>-18</v>
+        <v>0.6</v>
       </c>
       <c r="G3" t="n">
-        <v>-22</v>
+        <v>1</v>
       </c>
       <c r="H3" t="n">
-        <v>-17</v>
+        <v>0.7</v>
       </c>
       <c r="I3" t="n">
-        <v>93</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4">
@@ -462,28 +462,28 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>0.7</v>
+        <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>45</v>
+        <v>16</v>
       </c>
       <c r="D4" t="n">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="E4" t="n">
-        <v>46</v>
+        <v>21</v>
       </c>
       <c r="F4" t="n">
-        <v>-5</v>
+        <v>0.6</v>
       </c>
       <c r="G4" t="n">
-        <v>-19</v>
+        <v>1.1</v>
       </c>
       <c r="H4" t="n">
-        <v>-13</v>
+        <v>0.8</v>
       </c>
       <c r="I4" t="n">
-        <v>98</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5">
@@ -491,28 +491,28 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
+        <v>-6</v>
+      </c>
+      <c r="C5" t="n">
         <v>1</v>
       </c>
-      <c r="C5" t="n">
-        <v>67</v>
-      </c>
       <c r="D5" t="n">
-        <v>67</v>
+        <v>9</v>
       </c>
       <c r="E5" t="n">
-        <v>67</v>
+        <v>5</v>
       </c>
       <c r="F5" t="n">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="G5" t="n">
-        <v>-8</v>
+        <v>1</v>
       </c>
       <c r="H5" t="n">
-        <v>-5</v>
+        <v>0.7</v>
       </c>
       <c r="I5" t="n">
-        <v>100</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6">
@@ -520,28 +520,28 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>0.7</v>
+        <v>-2</v>
       </c>
       <c r="C6" t="n">
-        <v>55</v>
+        <v>5</v>
       </c>
       <c r="D6" t="n">
-        <v>55</v>
+        <v>9</v>
       </c>
       <c r="E6" t="n">
-        <v>55</v>
+        <v>8</v>
       </c>
       <c r="F6" t="n">
-        <v>-19</v>
+        <v>0.6</v>
       </c>
       <c r="G6" t="n">
-        <v>-13</v>
+        <v>0.9</v>
       </c>
       <c r="H6" t="n">
-        <v>-15</v>
+        <v>0.8</v>
       </c>
       <c r="I6" t="n">
-        <v>81</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7">
@@ -549,28 +549,28 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C7" t="n">
-        <v>51</v>
+        <v>11</v>
       </c>
       <c r="D7" t="n">
-        <v>51</v>
+        <v>20</v>
       </c>
       <c r="E7" t="n">
-        <v>51</v>
+        <v>15</v>
       </c>
       <c r="F7" t="n">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="G7" t="n">
-        <v>0</v>
+        <v>1.1</v>
       </c>
       <c r="H7" t="n">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="I7" t="n">
-        <v>60</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>